<commit_message>
code after midifying penalties/fixing assignements and new population generation
</commit_message>
<xml_diff>
--- a/results_loading_times/instance_10_times.xlsx
+++ b/results_loading_times/instance_10_times.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,30 +457,30 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C2" t="n">
         <v>5</v>
       </c>
       <c r="D2" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="n">
+        <v>4</v>
+      </c>
+      <c r="C3" t="n">
+        <v>5</v>
+      </c>
+      <c r="D3" t="n">
         <v>6</v>
-      </c>
-      <c r="C3" t="n">
-        <v>11</v>
-      </c>
-      <c r="D3" t="n">
-        <v>12</v>
       </c>
     </row>
     <row r="4">
@@ -488,41 +488,55 @@
         <v>5</v>
       </c>
       <c r="B4" t="n">
+        <v>5</v>
+      </c>
+      <c r="C4" t="n">
+        <v>5</v>
+      </c>
+      <c r="D4" t="n">
         <v>6</v>
-      </c>
-      <c r="C4" t="n">
-        <v>17</v>
-      </c>
-      <c r="D4" t="n">
-        <v>18</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C5" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D5" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B6" t="n">
         <v>7</v>
       </c>
       <c r="C6" t="n">
+        <v>5</v>
+      </c>
+      <c r="D6" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>3</v>
+      </c>
+      <c r="B7" t="n">
+        <v>7</v>
+      </c>
+      <c r="C7" t="n">
+        <v>11</v>
+      </c>
+      <c r="D7" t="n">
         <v>12</v>
-      </c>
-      <c r="D6" t="n">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>